<commit_message>
fixed directory access and now random list can append
</commit_message>
<xml_diff>
--- a/projects/sample_project/output/SampleBook1_anon.xlsx
+++ b/projects/sample_project/output/SampleBook1_anon.xlsx
@@ -460,7 +460,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -476,174 +476,158 @@
     <col max="6" width="9.10" min="6"/>
     <col max="7" width="9.10" min="7"/>
     <col max="8" width="9.10" min="8"/>
-    <col max="9" width="9.10" min="9"/>
   </cols>
   <sheetData>
-    <row spans="1:9" r="1">
+    <row spans="1:8" r="1">
+      <c r="A1" t="s" s="1">
+        <v>19</v>
+      </c>
       <c r="B1" t="s" s="1">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s" s="1">
         <v>5</v>
       </c>
     </row>
-    <row spans="1:9" r="2">
-      <c r="A2" t="n" s="1">
+    <row spans="1:8" r="2">
+      <c r="A2" t="n">
+        <v>12345678.0</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>12345678.0</v>
-      </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
         <v>14</v>
       </c>
+      <c r="E2" t="n">
+        <v>101.0</v>
+      </c>
       <c r="F2" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:8" r="3">
+      <c r="A3" t="n">
+        <v>23456789.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="n">
         <v>101.0</v>
       </c>
-      <c r="G2" t="n">
-        <v>82.0</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="F3" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="G3" t="s">
         <v>27</v>
       </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row spans="1:9" r="3">
-      <c r="A3" t="n" s="1">
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row spans="1:8" r="4">
+      <c r="A4" t="n">
+        <v>34567890.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row spans="1:8" r="5">
+      <c r="A5" t="n">
+        <v>10101010.0</v>
+      </c>
+      <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>23456789.0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row spans="1:8" r="6">
+      <c r="A6" t="n">
+        <v>23674567.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="n">
-        <v>101.0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>75.0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row spans="1:9" r="4">
-      <c r="A4" t="n" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>34567890.0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="n">
-        <v>101.0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row spans="1:9" r="5">
-      <c r="A5" t="n" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>10101010.0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="n">
+      <c r="E6" t="n">
         <v>102.0</v>
       </c>
-      <c r="G5" t="n">
-        <v>90.0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row spans="1:9" r="6">
-      <c r="A6" t="n" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>23674567.0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
       <c r="F6" t="n">
-        <v>102.0</v>
-      </c>
-      <c r="G6" t="n">
         <v>68.0</v>
       </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
       <c r="H6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -656,7 +640,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -667,73 +651,60 @@
     <col max="1" width="9.10" min="1"/>
     <col max="2" width="9.10" min="2"/>
     <col max="3" width="9.10" min="3"/>
-    <col max="4" width="9.10" min="4"/>
   </cols>
   <sheetData>
-    <row spans="1:4" r="1">
+    <row spans="1:3" r="1">
+      <c r="A1" t="s" s="1">
+        <v>19</v>
+      </c>
       <c r="B1" t="s" s="1">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s" s="1">
         <v>22</v>
       </c>
     </row>
-    <row spans="1:4" r="2">
-      <c r="A2" t="n" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
+    <row spans="1:3" r="2">
+      <c r="A2" t="n">
         <v>12345678.0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="n">
+      <c r="C2" t="n">
         <v>23.0</v>
       </c>
     </row>
-    <row spans="1:4" r="3">
-      <c r="A3" t="n" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
+    <row spans="1:3" r="3">
+      <c r="A3" t="n">
         <v>23456789.0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="n">
+      <c r="C3" t="n">
         <v>24.0</v>
       </c>
     </row>
-    <row spans="1:4" r="4">
-      <c r="A4" t="n" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
+    <row spans="1:3" r="4">
+      <c r="A4" t="n">
         <v>34567890.0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="n">
+      <c r="C4" t="n">
         <v>10.0</v>
       </c>
     </row>
-    <row spans="1:4" r="5">
-      <c r="A5" t="n" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
+    <row spans="1:3" r="5">
+      <c r="A5" t="n">
         <v>10101010.0</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="n">
+      <c r="C5" t="n">
         <v>16.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
First simple working version
Category detail is simple (ID, drop or non-ID) and the column
confirmation/adjusting routine is currently avoided.  Non-data sheets
are not handled in the output.  Anonymization of files works, otherwise,
and the sample output files here are correct (except for missing blank
sheet).
</commit_message>
<xml_diff>
--- a/projects/sample_project/output/SampleBook1_anon.xlsx
+++ b/projects/sample_project/output/SampleBook1_anon.xlsx
@@ -16,22 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
-  <si>
-    <t>Ard</t>
-  </si>
-  <si>
-    <t>Bar</t>
-  </si>
-  <si>
-    <t>Baz</t>
-  </si>
-  <si>
-    <t>Blarg</t>
-  </si>
-  <si>
-    <t>Broy</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Comment</t>
   </si>
@@ -45,9 +30,6 @@
     <t>First Name</t>
   </si>
   <si>
-    <t>Foo</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -66,28 +48,16 @@
     <t>Messy "things" here %.</t>
   </si>
   <si>
-    <t>Ploy</t>
-  </si>
-  <si>
     <t>Prereq?</t>
   </si>
   <si>
-    <t>Roy</t>
-  </si>
-  <si>
     <t>STDID</t>
   </si>
   <si>
     <t>Secion</t>
   </si>
   <si>
-    <t>Slab Drab</t>
-  </si>
-  <si>
     <t>TestScore</t>
-  </si>
-  <si>
-    <t>Wrest-Loy</t>
   </si>
   <si>
     <t>begagel begagel</t>
@@ -480,42 +450,42 @@
   <sheetData>
     <row spans="1:8" r="1">
       <c r="A1" t="s" s="1">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="1">
         <v>10</v>
       </c>
-      <c r="E1" t="s" s="1">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s" s="1">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s" s="1">
-        <v>17</v>
-      </c>
       <c r="H1" t="s" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row spans="1:8" r="2">
       <c r="A2" t="n">
-        <v>12345678.0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
+        <v>674920753</v>
+      </c>
+      <c r="B2" t="n">
+        <v>674920753</v>
+      </c>
+      <c r="C2" t="n">
+        <v>674920753</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E2" t="n">
         <v>101.0</v>
@@ -524,24 +494,24 @@
         <v>82.0</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row spans="1:8" r="3">
       <c r="A3" t="n">
-        <v>23456789.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
+        <v>406378728</v>
+      </c>
+      <c r="B3" t="n">
+        <v>406378728</v>
+      </c>
+      <c r="C3" t="n">
+        <v>406378728</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
         <v>101.0</v>
@@ -550,24 +520,24 @@
         <v>75.0</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row spans="1:8" r="4">
       <c r="A4" t="n">
-        <v>34567890.0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
+        <v>852158896</v>
+      </c>
+      <c r="B4" t="n">
+        <v>852158896</v>
+      </c>
+      <c r="C4" t="n">
+        <v>852158896</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n">
         <v>101.0</v>
@@ -576,24 +546,24 @@
         <v>41.0</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row spans="1:8" r="5">
       <c r="A5" t="n">
-        <v>10101010.0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
+        <v>123456789</v>
+      </c>
+      <c r="B5" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="C5" t="n">
+        <v>123456789</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E5" t="n">
         <v>102.0</v>
@@ -602,21 +572,21 @@
         <v>90.0</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row spans="1:8" r="6">
       <c r="A6" t="n">
-        <v>23674567.0</v>
-      </c>
-      <c r="B6" t="s">
+        <v>349854278</v>
+      </c>
+      <c r="B6" t="n">
+        <v>349854278</v>
+      </c>
+      <c r="C6" t="n">
+        <v>349854278</v>
+      </c>
+      <c r="D6" t="s">
         <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
       </c>
       <c r="E6" t="n">
         <v>102.0</v>
@@ -625,10 +595,10 @@
         <v>68.0</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -655,21 +625,21 @@
   <sheetData>
     <row spans="1:3" r="1">
       <c r="A1" t="s" s="1">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row spans="1:3" r="2">
       <c r="A2" t="n">
-        <v>12345678.0</v>
+        <v>674920753</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C2" t="n">
         <v>23.0</v>
@@ -677,10 +647,10 @@
     </row>
     <row spans="1:3" r="3">
       <c r="A3" t="n">
-        <v>23456789.0</v>
+        <v>406378728</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C3" t="n">
         <v>24.0</v>
@@ -688,10 +658,10 @@
     </row>
     <row spans="1:3" r="4">
       <c r="A4" t="n">
-        <v>34567890.0</v>
+        <v>852158896</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C4" t="n">
         <v>10.0</v>
@@ -699,10 +669,10 @@
     </row>
     <row spans="1:3" r="5">
       <c r="A5" t="n">
-        <v>10101010.0</v>
+        <v>123456789</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C5" t="n">
         <v>16.0</v>

</xml_diff>